<commit_message>
Cria módulo para leitura e manipulação no Excel, utilizando a biblioteca openpyxl.
</commit_message>
<xml_diff>
--- a/Controle_Financeiro.xlsx
+++ b/Controle_Financeiro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcon\ProjetoControleFinanceiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84F0010-9BD5-4962-A24B-18DCEA8D7348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB597F5-D621-4277-9DA5-6DEB30CAE2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENTRADAS" sheetId="1" r:id="rId1"/>
@@ -22,56 +22,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+  <si>
+    <t>Mês</t>
+  </si>
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Forma de Pagamento</t>
+  </si>
+  <si>
+    <t>Valor Total</t>
+  </si>
+  <si>
+    <t>Parcelado?</t>
+  </si>
+  <si>
+    <t>Total Parcelas</t>
+  </si>
+  <si>
+    <t>Entradas</t>
+  </si>
+  <si>
+    <t>Gastos</t>
+  </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mês </t>
+  </si>
   <si>
     <t>Dia</t>
   </si>
   <si>
-    <t>Mês</t>
-  </si>
-  <si>
-    <t>Ano</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Categoria</t>
-  </si>
-  <si>
     <t>Valor</t>
   </si>
   <si>
-    <t>Forma de Pagamento</t>
-  </si>
-  <si>
-    <t>Valor Total</t>
-  </si>
-  <si>
-    <t>Parcelado?</t>
-  </si>
-  <si>
-    <t>Nº Parcela</t>
-  </si>
-  <si>
-    <t>Total Parcelas</t>
-  </si>
-  <si>
-    <t>Entradas</t>
-  </si>
-  <si>
-    <t>Gastos</t>
-  </si>
-  <si>
-    <t>Saldo</t>
+    <t>Numero de Parcelas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -99,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,42 +450,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -489,50 +507,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -557,19 +577,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fluxo de cadastro de entradas no main.py
</commit_message>
<xml_diff>
--- a/Controle_Financeiro.xlsx
+++ b/Controle_Financeiro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcon\ProjetoControleFinanceiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB597F5-D621-4277-9DA5-6DEB30CAE2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C551A976-8D2C-4C95-B12B-ADEC056C33E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENTRADAS" sheetId="1" r:id="rId1"/>
@@ -24,30 +24,45 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mês </t>
+  </si>
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Forma de Pagamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia </t>
+  </si>
+  <si>
+    <t>Valor Total</t>
+  </si>
+  <si>
+    <t>Parcelado?</t>
+  </si>
+  <si>
+    <t>Numero de Parcelas</t>
+  </si>
+  <si>
+    <t>Total Parcelas</t>
+  </si>
+  <si>
     <t>Mês</t>
   </si>
   <si>
-    <t>Ano</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Categoria</t>
-  </si>
-  <si>
-    <t>Forma de Pagamento</t>
-  </si>
-  <si>
-    <t>Valor Total</t>
-  </si>
-  <si>
-    <t>Parcelado?</t>
-  </si>
-  <si>
-    <t>Total Parcelas</t>
-  </si>
-  <si>
     <t>Entradas</t>
   </si>
   <si>
@@ -55,21 +70,6 @@
   </si>
   <si>
     <t>Saldo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mês </t>
-  </si>
-  <si>
-    <t>Dia</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>Numero de Parcelas</t>
   </si>
 </sst>
 </file>
@@ -452,39 +452,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -507,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -525,34 +525,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -577,19 +577,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fluxo de cadastro de gastos com parcelamento real com uma linha por parcela
</commit_message>
<xml_diff>
--- a/Controle_Financeiro.xlsx
+++ b/Controle_Financeiro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcon\ProjetoControleFinanceiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C551A976-8D2C-4C95-B12B-ADEC056C33E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6904D46C-BF0F-4144-BFCC-CA7E4A8F617B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENTRADAS" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>Valor Total</t>
   </si>
   <si>
-    <t>Parcelado?</t>
-  </si>
-  <si>
-    <t>Numero de Parcelas</t>
-  </si>
-  <si>
-    <t>Total Parcelas</t>
+    <t>Parcelado</t>
+  </si>
+  <si>
+    <t>Numero  Parcelas</t>
+  </si>
+  <si>
+    <t>Valor Parcela</t>
   </si>
   <si>
     <t>Mês</t>
@@ -450,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,6 +490,7 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E5" s="1"/>
     </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -507,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Refatora excel_manager removendo salvamento e ajustando escrita de entradas e gastos
</commit_message>
<xml_diff>
--- a/Controle_Financeiro.xlsx
+++ b/Controle_Financeiro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcon\ProjetoControleFinanceiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6904D46C-BF0F-4144-BFCC-CA7E4A8F617B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EBC58F-2EF1-4FE3-8C1F-B605AC072B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Numero  Parcelas</t>
   </si>
   <si>
-    <t>Valor Parcela</t>
-  </si>
-  <si>
     <t>Mês</t>
   </si>
   <si>
@@ -70,6 +67,9 @@
   </si>
   <si>
     <t>Saldo</t>
+  </si>
+  <si>
+    <t>Valor  Parcela</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -578,19 +578,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementa parcelamento real de gastos com controle por parcela
</commit_message>
<xml_diff>
--- a/Controle_Financeiro.xlsx
+++ b/Controle_Financeiro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcon\ProjetoControleFinanceiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EBC58F-2EF1-4FE3-8C1F-B605AC072B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDD2B1-E561-41C5-9786-68704235032C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,6 +57,9 @@
     <t>Numero  Parcelas</t>
   </si>
   <si>
+    <t>Valor  Parcela</t>
+  </si>
+  <si>
     <t>Mês</t>
   </si>
   <si>
@@ -67,9 +70,6 @@
   </si>
   <si>
     <t>Saldo</t>
-  </si>
-  <si>
-    <t>Valor  Parcela</t>
   </si>
 </sst>
 </file>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,9 +553,12 @@
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -578,19 +581,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrige contrato de dados e finaliza fluxo de gastos parcelados
</commit_message>
<xml_diff>
--- a/Controle_Financeiro.xlsx
+++ b/Controle_Financeiro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcon\ProjetoControleFinanceiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDD2B1-E561-41C5-9786-68704235032C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215CEAE9-72B0-45A5-878A-28E48C52ECA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENTRADAS" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,10 +488,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E5" s="1"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -506,10 +509,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,9 +559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">

</xml_diff>

<commit_message>
Move as regras de negócio para services.finace simplificando main
</commit_message>
<xml_diff>
--- a/Controle_Financeiro.xlsx
+++ b/Controle_Financeiro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcon\ProjetoControleFinanceiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215CEAE9-72B0-45A5-878A-28E48C52ECA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B862D3E-8BD8-49DE-AADF-2264C8E56DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -451,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,7 +465,7 @@
     <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,11 +487,9 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E4" s="1"/>
     </row>
   </sheetData>
@@ -509,10 +507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +557,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">

</xml_diff>

<commit_message>
feat: menu com registro de entradas, gastos, resumo mensal e saldo
</commit_message>
<xml_diff>
--- a/Controle_Financeiro.xlsx
+++ b/Controle_Financeiro.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="32340" yWindow="1530" windowWidth="15375" windowHeight="7725" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="32340" yWindow="1530" windowWidth="15375" windowHeight="7725" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ENTRADAS" sheetId="1" state="visible" r:id="rId1"/>
@@ -448,7 +448,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -627,7 +627,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Presente</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -640,7 +640,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pix</t>
+          <t>Débito</t>
         </is>
       </c>
       <c r="H2" t="b">
@@ -659,7 +659,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Presente (1/3)</t>
+          <t>Shopping (1/3)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -697,7 +697,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Presente (2/3)</t>
+          <t>Shopping (2/3)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -735,7 +735,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Presente (3/3)</t>
+          <t>Shopping (3/3)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -779,7 +779,7 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>